<commit_message>
improve: refactor statistic data
</commit_message>
<xml_diff>
--- a/estatisticas_q.xlsx
+++ b/estatisticas_q.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>n_agregados</t>
+          <t>n_contornos</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -452,6 +452,16 @@
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>desvio_padrao_q</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>min_q</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>max_q</t>
         </is>
       </c>
     </row>
@@ -470,6 +480,12 @@
       <c r="D2" t="n">
         <v>0.001508392141650155</v>
       </c>
+      <c r="E2" t="n">
+        <v>2.304e-05</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.01538384</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -486,6 +502,12 @@
       <c r="D3" t="n">
         <v>0.0007460063978545818</v>
       </c>
+      <c r="E3" t="n">
+        <v>2.056e-05</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.00589112</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -502,6 +524,12 @@
       <c r="D4" t="n">
         <v>0.0009236067001152469</v>
       </c>
+      <c r="E4" t="n">
+        <v>7.76e-06</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0084864</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -518,6 +546,12 @@
       <c r="D5" t="n">
         <v>0.001225617044961392</v>
       </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.01146816</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -534,6 +568,12 @@
       <c r="D6" t="n">
         <v>0.001182187736745572</v>
       </c>
+      <c r="E6" t="n">
+        <v>3.456e-05</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.01113464</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -550,6 +590,12 @@
       <c r="D7" t="n">
         <v>0.001076197903932554</v>
       </c>
+      <c r="E7" t="n">
+        <v>3.24e-05</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0109924</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -566,6 +612,12 @@
       <c r="D8" t="n">
         <v>0.001444794146446541</v>
       </c>
+      <c r="E8" t="n">
+        <v>5.072e-05</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.01420992</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -582,6 +634,12 @@
       <c r="D9" t="n">
         <v>0.001190354561515778</v>
       </c>
+      <c r="E9" t="n">
+        <v>5.552e-05</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.009123600000000001</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -598,6 +656,12 @@
       <c r="D10" t="n">
         <v>0.001341255073184956</v>
       </c>
+      <c r="E10" t="n">
+        <v>3.624e-05</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.008343359999999999</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -614,6 +678,12 @@
       <c r="D11" t="n">
         <v>0.0009897671900473077</v>
       </c>
+      <c r="E11" t="n">
+        <v>3.304e-05</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.00639712</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -630,6 +700,12 @@
       <c r="D12" t="n">
         <v>0.001237105874070238</v>
       </c>
+      <c r="E12" t="n">
+        <v>5.008e-05</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.009144319999999999</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -646,6 +722,12 @@
       <c r="D13" t="n">
         <v>0.0010231437509751</v>
       </c>
+      <c r="E13" t="n">
+        <v>5.424e-05</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.00627856</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -662,6 +744,12 @@
       <c r="D14" t="n">
         <v>0.0009975432709833343</v>
       </c>
+      <c r="E14" t="n">
+        <v>1.848e-05</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.008697760000000001</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -678,6 +766,12 @@
       <c r="D15" t="n">
         <v>0.001020251759943706</v>
       </c>
+      <c r="E15" t="n">
+        <v>2.344e-05</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.00897856</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -694,6 +788,12 @@
       <c r="D16" t="n">
         <v>0.001125855131378662</v>
       </c>
+      <c r="E16" t="n">
+        <v>1.616e-05</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.01161448</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -710,6 +810,12 @@
       <c r="D17" t="n">
         <v>0.001237412015190878</v>
       </c>
+      <c r="E17" t="n">
+        <v>1.736e-05</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.009345040000000001</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -725,6 +831,12 @@
       </c>
       <c r="D18" t="n">
         <v>0.0009524153289664622</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.496e-05</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.00642688</v>
       </c>
     </row>
   </sheetData>

</xml_diff>